<commit_message>
Fixed minor formatting issues
</commit_message>
<xml_diff>
--- a/tables/S1_Table.xlsx
+++ b/tables/S1_Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
   <si>
     <t>Station</t>
   </si>
@@ -77,9 +77,6 @@
     <t>TSS (mg/L)</t>
   </si>
   <si>
-    <t>Fluorescence(mg/m3)</t>
-  </si>
-  <si>
     <t>PAR</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Temperature ©</t>
-  </si>
-  <si>
     <t>TDS (mg/L)</t>
   </si>
   <si>
@@ -204,6 +198,9 @@
   </si>
   <si>
     <t>C) Inland Lake Survey Samples</t>
+  </si>
+  <si>
+    <t>Fluorescence (mg/m3)</t>
   </si>
 </sst>
 </file>
@@ -426,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -490,6 +487,11 @@
     <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,14 +809,34 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
@@ -869,16 +891,16 @@
       <c r="R2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="31" t="s">
         <v>17</v>
-      </c>
-      <c r="T2" s="31" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B3" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="8">
         <v>43.188055560000002</v>
@@ -887,7 +909,7 @@
         <v>86.343888890000002</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="7">
         <v>11</v>
@@ -937,7 +959,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B4" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="11">
         <v>43.199722219999998</v>
@@ -946,7 +968,7 @@
         <v>86.569722220000003</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="10">
         <v>10</v>
@@ -999,7 +1021,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="13">
         <v>3</v>
@@ -1049,7 +1071,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B6" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>43.240965000000003</v>
@@ -1058,7 +1080,7 @@
         <v>86.278964999999999</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="15">
         <v>9</v>
@@ -1073,31 +1095,31 @@
         <v>8.6385699999999996</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S6">
         <v>14.23325</v>
@@ -1111,7 +1133,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="16">
         <v>6</v>
@@ -1126,31 +1148,31 @@
         <v>0</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S7" s="13">
         <v>13.111750000000001</v>
@@ -1161,7 +1183,7 @@
     </row>
     <row r="9" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="56" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
@@ -1184,57 +1206,57 @@
         <v>5</v>
       </c>
       <c r="H10" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="K10" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>28</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>8</v>
       </c>
       <c r="M10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="P10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="Q10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="20" t="s">
+      <c r="R10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="Q10" s="20" t="s">
+      <c r="S10" s="20" t="s">
         <v>33</v>
-      </c>
-      <c r="R10" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="S10" s="20" t="s">
-        <v>35</v>
       </c>
       <c r="T10" s="20" t="s">
         <v>9</v>
       </c>
       <c r="U10" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="V10" s="20" t="s">
         <v>7</v>
       </c>
       <c r="W10" s="37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="10">
         <v>43.252079999999999</v>
@@ -1243,7 +1265,7 @@
         <v>86.252420000000001</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="10">
         <v>6</v>
@@ -1305,7 +1327,7 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="13">
         <v>6</v>
@@ -1365,7 +1387,7 @@
     </row>
     <row r="13" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="27">
         <v>43.238610999999999</v>
@@ -1374,7 +1396,7 @@
         <v>86.299166999999997</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="10">
         <v>4</v>
@@ -1436,7 +1458,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="13">
         <v>4</v>
@@ -1496,7 +1518,7 @@
     </row>
     <row r="15" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="10">
         <v>43.232970000000002</v>
@@ -1505,7 +1527,7 @@
         <v>86.326840000000004</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="10">
         <v>6</v>
@@ -1567,7 +1589,7 @@
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="13">
         <v>6</v>
@@ -1627,7 +1649,7 @@
     </row>
     <row r="17" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="26">
         <v>43.223059999999997</v>
@@ -1636,7 +1658,7 @@
         <v>86.298090000000002</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="10">
         <v>6</v>
@@ -1698,7 +1720,7 @@
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F18" s="13">
         <v>6</v>
@@ -1758,13 +1780,13 @@
     </row>
     <row r="20" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="56"/>
       <c r="B21" s="28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>1</v>
@@ -1773,7 +1795,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F21" s="17" t="s">
         <v>3</v>
@@ -1788,10 +1810,10 @@
         <v>8</v>
       </c>
       <c r="J21" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L21" s="20" t="s">
         <v>9</v>
@@ -1799,13 +1821,13 @@
       <c r="M21" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N21" s="19" t="s">
-        <v>44</v>
+      <c r="N21" s="57" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="10">
         <v>42.811630000000001</v>
@@ -1817,7 +1839,7 @@
         <v>51.5</v>
       </c>
       <c r="F22" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" s="40">
         <v>6</v>
@@ -1845,7 +1867,7 @@
         <f>(4.56+4.12+4.74)/3</f>
         <v>4.4733333333333336</v>
       </c>
-      <c r="N22" s="41">
+      <c r="N22" s="58">
         <f>(11.42+13.95+21)/3</f>
         <v>15.456666666666665</v>
       </c>
@@ -1856,7 +1878,7 @@
       <c r="D23" s="16"/>
       <c r="E23" s="45"/>
       <c r="F23" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23" s="25">
         <v>2</v>
@@ -1879,13 +1901,13 @@
       <c r="M23" s="46">
         <v>17.29</v>
       </c>
-      <c r="N23" s="46">
+      <c r="N23" s="59">
         <v>730.43</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C24" s="22">
         <v>42.501390000000001</v>
@@ -1897,7 +1919,7 @@
         <v>56</v>
       </c>
       <c r="F24" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G24" s="40">
         <v>6</v>
@@ -1924,7 +1946,7 @@
         <f>(4.05+4.39+4.73)/3</f>
         <v>4.3899999999999997</v>
       </c>
-      <c r="N24" s="41">
+      <c r="N24" s="58">
         <f>(8.69+9.22+11.25)/3</f>
         <v>9.7200000000000006</v>
       </c>
@@ -1935,7 +1957,7 @@
       <c r="D25" s="16"/>
       <c r="E25" s="45"/>
       <c r="F25" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G25" s="25">
         <v>2</v>
@@ -1958,13 +1980,13 @@
       <c r="M25" s="46">
         <v>16.7</v>
       </c>
-      <c r="N25" s="46">
+      <c r="N25" s="59">
         <v>1056.53</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="15">
         <v>42.419409999999999</v>
@@ -1976,7 +1998,7 @@
         <v>49.8</v>
       </c>
       <c r="F26" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G26" s="40">
         <v>10</v>
@@ -2004,7 +2026,7 @@
         <f>(4.32+4.19+3.87+2.17+3.1)/5</f>
         <v>3.5300000000000002</v>
       </c>
-      <c r="N26" s="41">
+      <c r="N26" s="58">
         <f>(17.82+19.83+34.29+57.17+71.89)/5</f>
         <v>40.200000000000003</v>
       </c>
@@ -2015,7 +2037,7 @@
       <c r="D27" s="16"/>
       <c r="E27" s="49"/>
       <c r="F27" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="50">
         <v>6</v>
@@ -2043,14 +2065,14 @@
         <f>(5.23+3.1+2.43)/3</f>
         <v>3.5866666666666664</v>
       </c>
-      <c r="N27" s="51">
+      <c r="N27" s="60">
         <f>(441.76+71.89+807.64)/3</f>
         <v>440.43</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="52">
         <v>42.315010000000001</v>
@@ -2062,7 +2084,7 @@
         <v>24.6</v>
       </c>
       <c r="F28" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G28" s="40">
         <v>6</v>
@@ -2090,7 +2112,7 @@
         <f>(4+4.7+5.72)/3</f>
         <v>4.8066666666666658</v>
       </c>
-      <c r="N28" s="41">
+      <c r="N28" s="58">
         <f>(14.66+222.6+4.13)/3</f>
         <v>80.463333333333324</v>
       </c>
@@ -2101,7 +2123,7 @@
       <c r="D29" s="16"/>
       <c r="E29" s="45"/>
       <c r="F29" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G29" s="25">
         <v>2</v>
@@ -2124,13 +2146,13 @@
       <c r="M29" s="46">
         <v>5.13</v>
       </c>
-      <c r="N29" s="46">
+      <c r="N29" s="59">
         <v>216.38</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C30" s="15">
         <v>42.420140000000004</v>
@@ -2142,7 +2164,7 @@
         <v>88</v>
       </c>
       <c r="F30" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G30" s="40">
         <v>6</v>
@@ -2170,7 +2192,7 @@
         <f>(8.79+7.71+8.35)/3</f>
         <v>8.2833333333333332</v>
       </c>
-      <c r="N30" s="41">
+      <c r="N30" s="58">
         <f>(7.73+5.14+9.31)/3</f>
         <v>7.3933333333333335</v>
       </c>
@@ -2181,7 +2203,7 @@
       <c r="D31" s="16"/>
       <c r="E31" s="45"/>
       <c r="F31" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31" s="25">
         <v>2</v>
@@ -2204,13 +2226,13 @@
       <c r="M31" s="46">
         <v>111.21</v>
       </c>
-      <c r="N31" s="46">
+      <c r="N31" s="59">
         <v>296.23</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C32" s="15">
         <v>42.808799999999998</v>
@@ -2222,7 +2244,7 @@
         <v>42.9</v>
       </c>
       <c r="F32" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G32" s="40">
         <v>6</v>
@@ -2250,7 +2272,7 @@
         <f>(3.86+3.82+3.59)/3</f>
         <v>3.7566666666666664</v>
       </c>
-      <c r="N32" s="41">
+      <c r="N32" s="58">
         <f>(5.66+5.6+9.88)/3</f>
         <v>7.0466666666666669</v>
       </c>
@@ -2261,7 +2283,7 @@
       <c r="D33" s="25"/>
       <c r="E33" s="45"/>
       <c r="F33" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G33" s="25">
         <v>2</v>
@@ -2284,13 +2306,13 @@
       <c r="M33" s="46">
         <v>4.41</v>
       </c>
-      <c r="N33" s="46">
+      <c r="N33" s="59">
         <v>588.12</v>
       </c>
     </row>
     <row r="34" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C34" s="52">
         <v>42.405349999999999</v>
@@ -2302,7 +2324,7 @@
         <v>36</v>
       </c>
       <c r="F34" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G34" s="23">
         <v>10</v>
@@ -2330,7 +2352,7 @@
         <f>(5.96+5.4+5.93+2.79+4.7)/5</f>
         <v>4.9559999999999995</v>
       </c>
-      <c r="N34" s="55">
+      <c r="N34" s="61">
         <f>(10.2+4.95+8.43+41.59+10.03)</f>
         <v>75.2</v>
       </c>
@@ -2341,7 +2363,7 @@
       <c r="D35" s="50"/>
       <c r="E35" s="49"/>
       <c r="F35" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G35" s="50">
         <v>6</v>
@@ -2369,14 +2391,14 @@
         <f>(2.81+5.08+4.91)/3</f>
         <v>4.2666666666666666</v>
       </c>
-      <c r="N35" s="51">
+      <c r="N35" s="60">
         <f>(77.87+8.95+249.87)/3</f>
         <v>112.23</v>
       </c>
     </row>
     <row r="36" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C36" s="22">
         <v>42.788510000000002</v>
@@ -2388,7 +2410,7 @@
         <v>83</v>
       </c>
       <c r="F36" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G36" s="40">
         <v>6</v>
@@ -2415,7 +2437,7 @@
         <f>(5.29+5.74+6.8)/3</f>
         <v>5.9433333333333342</v>
       </c>
-      <c r="N36" s="41">
+      <c r="N36" s="58">
         <f>(4.94+3.55+6.04)/3</f>
         <v>4.8433333333333337</v>
       </c>
@@ -2426,7 +2448,7 @@
       <c r="D37" s="25"/>
       <c r="E37" s="45"/>
       <c r="F37" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G37" s="25">
         <v>2</v>
@@ -2449,13 +2471,13 @@
       <c r="M37" s="46">
         <v>44.68</v>
       </c>
-      <c r="N37" s="46">
+      <c r="N37" s="59">
         <v>116.47</v>
       </c>
     </row>
     <row r="38" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="53" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="22">
         <v>42.393419999999999</v>
@@ -2467,7 +2489,7 @@
         <v>52.2</v>
       </c>
       <c r="F38" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G38" s="23">
         <v>10</v>
@@ -2495,7 +2517,7 @@
         <f>(3.95+5.02+5.88+4.31+3.42)/5</f>
         <v>4.516</v>
       </c>
-      <c r="N38" s="55">
+      <c r="N38" s="61">
         <f>(1.3+2.98+4.22+4.78+10.41)/5</f>
         <v>4.7380000000000004</v>
       </c>
@@ -2506,7 +2528,7 @@
       <c r="D39" s="50"/>
       <c r="E39" s="49"/>
       <c r="F39" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G39" s="50">
         <v>4</v>
@@ -2534,14 +2556,14 @@
         <f>(5.93+6.82)/2</f>
         <v>6.375</v>
       </c>
-      <c r="N39" s="51">
+      <c r="N39" s="60">
         <f>(9.65+556.58)/2</f>
         <v>283.11500000000001</v>
       </c>
     </row>
     <row r="40" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="38" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C40" s="15">
         <v>42.044429999999998</v>
@@ -2553,7 +2575,7 @@
         <v>37.200000000000003</v>
       </c>
       <c r="F40" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G40" s="40">
         <v>6</v>
@@ -2581,7 +2603,7 @@
         <f>(3.1+2.68+4.02)/3</f>
         <v>3.2666666666666671</v>
       </c>
-      <c r="N40" s="41">
+      <c r="N40" s="58">
         <f>(3.89+2.59+3.97)/3</f>
         <v>3.4833333333333338</v>
       </c>
@@ -2592,7 +2614,7 @@
       <c r="D41" s="25"/>
       <c r="E41" s="45"/>
       <c r="F41" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G41" s="25">
         <v>2</v>
@@ -2615,13 +2637,13 @@
       <c r="M41" s="46">
         <v>3.74</v>
       </c>
-      <c r="N41" s="46">
+      <c r="N41" s="59">
         <v>81.48</v>
       </c>
     </row>
     <row r="42" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="53" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C42" s="15">
         <v>42.436390000000003</v>
@@ -2633,7 +2655,7 @@
         <v>61</v>
       </c>
       <c r="F42" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G42" s="23">
         <v>10</v>
@@ -2661,7 +2683,7 @@
         <f>(2.57+5.62+4.25+2.78+3.24)/5</f>
         <v>3.6920000000000002</v>
       </c>
-      <c r="N42" s="55">
+      <c r="N42" s="61">
         <f>(19.9+2.44+3.42+3.83+45.84)/5</f>
         <v>15.086000000000002</v>
       </c>
@@ -2672,7 +2694,7 @@
       <c r="D43" s="50"/>
       <c r="E43" s="49"/>
       <c r="F43" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G43" s="50">
         <v>6</v>
@@ -2700,14 +2722,14 @@
         <f>(3.86+3.57+3.41)/3</f>
         <v>3.6133333333333333</v>
       </c>
-      <c r="N43" s="51">
+      <c r="N43" s="60">
         <f>(105.29+77.69+66.08)/3</f>
         <v>83.02</v>
       </c>
     </row>
     <row r="44" spans="2:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" s="15">
         <v>42.55198</v>
@@ -2719,7 +2741,7 @@
         <v>32.6</v>
       </c>
       <c r="F44" s="40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G44" s="40">
         <v>6</v>
@@ -2747,7 +2769,7 @@
         <f>(4.96+4.99+5.76)/3</f>
         <v>5.2366666666666664</v>
       </c>
-      <c r="N44" s="41">
+      <c r="N44" s="58">
         <f>(3.66+7.86+11.48)/3</f>
         <v>7.666666666666667</v>
       </c>
@@ -2758,7 +2780,7 @@
       <c r="D45" s="25"/>
       <c r="E45" s="45"/>
       <c r="F45" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G45" s="25">
         <v>2</v>
@@ -2782,7 +2804,7 @@
       <c r="M45" s="46">
         <v>5.72</v>
       </c>
-      <c r="N45" s="46">
+      <c r="N45" s="59">
         <v>300.3</v>
       </c>
     </row>

</xml_diff>